<commit_message>
chart sudah ada tinggal pembenaran logikanya
</commit_message>
<xml_diff>
--- a/File Data OTA BRI FMS 01 Oktober 2024 - 18 Oktober 2024.xlsx
+++ b/File Data OTA BRI FMS 01 Oktober 2024 - 18 Oktober 2024.xlsx
@@ -135,6 +135,161 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="6667500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>20</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="6667500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>40</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="6667500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>60</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="6667500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>80</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="6667500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>100</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="6667500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -419,12 +574,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,7 +587,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
@@ -715,6 +870,16 @@
         <v>22290</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Total Populasi</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>201221</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
@@ -722,5 +887,6 @@
     <mergeCell ref="A13:E13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sudah menggunakan chart tinggal penataan yang perlu dirapikan
</commit_message>
<xml_diff>
--- a/File Data OTA BRI FMS 01 Oktober 2024 - 18 Oktober 2024.xlsx
+++ b/File Data OTA BRI FMS 01 Oktober 2024 - 18 Oktober 2024.xlsx
@@ -144,7 +144,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525000" cy="6667500"/>
+    <ext cx="9429750" cy="6562725"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -169,7 +169,7 @@
       <row>20</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525000" cy="6667500"/>
+    <ext cx="9429750" cy="6572250"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -194,7 +194,7 @@
       <row>40</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525000" cy="6667500"/>
+    <ext cx="9429750" cy="6562725"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -219,7 +219,7 @@
       <row>60</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525000" cy="6667500"/>
+    <ext cx="9429750" cy="6572250"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -244,7 +244,7 @@
       <row>80</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525000" cy="6667500"/>
+    <ext cx="9429750" cy="6562725"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -269,7 +269,7 @@
       <row>100</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9525000" cy="6667500"/>
+    <ext cx="9429750" cy="6572250"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -277,6 +277,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>120</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9429750" cy="6572250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -877,7 +902,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>201221</v>
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
perubahan pada warna dan ukuran gambar
</commit_message>
<xml_diff>
--- a/File Data OTA BRI FMS 01 Oktober 2024 - 18 Oktober 2024.xlsx
+++ b/File Data OTA BRI FMS 01 Oktober 2024 - 18 Oktober 2024.xlsx
@@ -144,7 +144,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9429750" cy="6562725"/>
+    <ext cx="3619500" cy="2714625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -169,7 +169,7 @@
       <row>20</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9429750" cy="6572250"/>
+    <ext cx="3619500" cy="2714625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -194,7 +194,7 @@
       <row>40</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9429750" cy="6562725"/>
+    <ext cx="3619500" cy="2714625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -219,7 +219,7 @@
       <row>60</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9429750" cy="6572250"/>
+    <ext cx="3619500" cy="2714625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -244,7 +244,7 @@
       <row>80</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9429750" cy="6562725"/>
+    <ext cx="3619500" cy="2714625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -269,7 +269,7 @@
       <row>100</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9429750" cy="6572250"/>
+    <ext cx="3619500" cy="2714625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -294,7 +294,7 @@
       <row>120</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9429750" cy="6572250"/>
+    <ext cx="3619500" cy="2714625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>

</xml_diff>

<commit_message>
penambahan chart sudah berhasil dan sudah rapi
</commit_message>
<xml_diff>
--- a/File Data OTA BRI FMS 01 Oktober 2024 - 18 Oktober 2024.xlsx
+++ b/File Data OTA BRI FMS 01 Oktober 2024 - 18 Oktober 2024.xlsx
@@ -139,9 +139,9 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>10</col>
+      <col>7</col>
       <colOff>0</colOff>
-      <row>0</row>
+      <row>1</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3619500" cy="2714625"/>
@@ -164,9 +164,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>10</col>
+      <col>14</col>
       <colOff>0</colOff>
-      <row>20</row>
+      <row>1</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3619500" cy="2714625"/>
@@ -189,9 +189,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>10</col>
+      <col>7</col>
       <colOff>0</colOff>
-      <row>40</row>
+      <row>18</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3619500" cy="2714625"/>
@@ -214,9 +214,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>10</col>
+      <col>14</col>
       <colOff>0</colOff>
-      <row>60</row>
+      <row>18</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3619500" cy="2714625"/>
@@ -239,9 +239,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>10</col>
+      <col>7</col>
       <colOff>0</colOff>
-      <row>80</row>
+      <row>34</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3619500" cy="2714625"/>
@@ -264,9 +264,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>10</col>
+      <col>14</col>
       <colOff>0</colOff>
-      <row>100</row>
+      <row>34</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3619500" cy="2714625"/>
@@ -289,9 +289,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>10</col>
+      <col>7</col>
       <colOff>0</colOff>
-      <row>120</row>
+      <row>50</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3619500" cy="2714625"/>
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,6 +617,8 @@
     <col width="37" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="13.44083333430558" customWidth="1" min="8" max="8"/>
+    <col width="13.44083333430558" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -625,8 +627,18 @@
           <t>TAMS SHARING 10.2.2.5:7000</t>
         </is>
       </c>
-    </row>
-    <row r="2">
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>1. Data Download Tams Sharing 10.2.2.5:7000</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>2. Data Apply Tams Sharing 10.2.2.5:7000</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="14.36309523792468" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Type</t>
@@ -653,7 +665,7 @@
         </is>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="14.36309523792468" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
           <t>A920pro</t>
@@ -672,7 +684,7 @@
         <v>6534</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="14.36309523792468" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
           <t>X990</t>
@@ -691,7 +703,7 @@
         <v>4611</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="14.36309523792468" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
           <t>Total</t>
@@ -710,15 +722,15 @@
         <v>11145</v>
       </c>
     </row>
-    <row r="6"/>
-    <row r="7">
+    <row r="6" ht="14.36309523792468" customHeight="1"/>
+    <row r="7" ht="14.36309523792468" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>TAMS FMS 10.2.30.2:7000</t>
         </is>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="14.36309523792468" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Type</t>
@@ -745,7 +757,7 @@
         </is>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="14.36309523792468" customHeight="1">
       <c r="A9" t="inlineStr">
         <is>
           <t>A920pro</t>
@@ -764,7 +776,7 @@
         <v>6534</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="14.36309523792468" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
           <t>X990</t>
@@ -783,7 +795,7 @@
         <v>4611</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="14.36309523792468" customHeight="1">
       <c r="A11" t="inlineStr">
         <is>
           <t>Total</t>
@@ -802,16 +814,16 @@
         <v>11145</v>
       </c>
     </row>
-    <row r="12"/>
-    <row r="13">
+    <row r="12" ht="14.36309523792468" customHeight="1"/>
+    <row r="13" ht="14.36309523792468" customHeight="1">
       <c r="A13" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">TAMS FMS dan SHARING </t>
         </is>
       </c>
     </row>
-    <row r="14"/>
-    <row r="15">
+    <row r="14" ht="14.36309523792468" customHeight="1"/>
+    <row r="15" ht="14.36309523792468" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
           <t>Type</t>
@@ -838,7 +850,7 @@
         </is>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="14.36309523792468" customHeight="1">
       <c r="A16" t="inlineStr">
         <is>
           <t>A920pro</t>
@@ -894,8 +906,19 @@
       <c r="E18" t="n">
         <v>22290</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="H18" s="2" t="inlineStr">
+        <is>
+          <t>3. Data Download Tams FMS 10.2.30.2:7000</t>
+        </is>
+      </c>
+      <c r="O18" s="2" t="inlineStr">
+        <is>
+          <t>4. Data Apply Tams FMS 10.2.30.2:7000</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="14.36309523792468" customHeight="1"/>
+    <row r="20" ht="14.36309523792468" customHeight="1">
       <c r="A20" t="inlineStr">
         <is>
           <t>Total Populasi</t>
@@ -905,6 +928,68 @@
         <v>30000</v>
       </c>
     </row>
+    <row r="21" ht="14.36309523792468" customHeight="1"/>
+    <row r="22" ht="14.36309523792468" customHeight="1"/>
+    <row r="23" ht="14.36309523792468" customHeight="1"/>
+    <row r="24" ht="14.36309523792468" customHeight="1"/>
+    <row r="25" ht="14.36309523792468" customHeight="1"/>
+    <row r="26" ht="14.36309523792468" customHeight="1"/>
+    <row r="27" ht="14.36309523792468" customHeight="1"/>
+    <row r="28" ht="14.36309523792468" customHeight="1"/>
+    <row r="29" ht="14.36309523792468" customHeight="1"/>
+    <row r="30" ht="14.36309523792468" customHeight="1"/>
+    <row r="31" ht="14.36309523792468" customHeight="1"/>
+    <row r="32" ht="14.36309523792468" customHeight="1"/>
+    <row r="33" ht="14.36309523792468" customHeight="1"/>
+    <row r="34">
+      <c r="H34" s="2" t="inlineStr">
+        <is>
+          <t>5. Data Download Tams FMS dan Sharing</t>
+        </is>
+      </c>
+      <c r="O34" s="2" t="inlineStr">
+        <is>
+          <t>6. Data Apply Tams FMS dan Sharing</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="14.36309523792468" customHeight="1"/>
+    <row r="36" ht="14.36309523792468" customHeight="1"/>
+    <row r="37" ht="14.36309523792468" customHeight="1"/>
+    <row r="38" ht="14.36309523792468" customHeight="1"/>
+    <row r="39" ht="14.36309523792468" customHeight="1"/>
+    <row r="40" ht="14.36309523792468" customHeight="1"/>
+    <row r="41" ht="14.36309523792468" customHeight="1"/>
+    <row r="42" ht="14.36309523792468" customHeight="1"/>
+    <row r="43" ht="14.36309523792468" customHeight="1"/>
+    <row r="44" ht="14.36309523792468" customHeight="1"/>
+    <row r="45" ht="14.36309523792468" customHeight="1"/>
+    <row r="46" ht="14.36309523792468" customHeight="1"/>
+    <row r="47" ht="14.36309523792468" customHeight="1"/>
+    <row r="48" ht="14.36309523792468" customHeight="1"/>
+    <row r="49" ht="14.36309523792468" customHeight="1"/>
+    <row r="50">
+      <c r="H50" s="2" t="inlineStr">
+        <is>
+          <t>7. Data Update Aplikasi Versi</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" ht="14.36309523792468" customHeight="1"/>
+    <row r="52" ht="14.36309523792468" customHeight="1"/>
+    <row r="53" ht="14.36309523792468" customHeight="1"/>
+    <row r="54" ht="14.36309523792468" customHeight="1"/>
+    <row r="55" ht="14.36309523792468" customHeight="1"/>
+    <row r="56" ht="14.36309523792468" customHeight="1"/>
+    <row r="57" ht="14.36309523792468" customHeight="1"/>
+    <row r="58" ht="14.36309523792468" customHeight="1"/>
+    <row r="59" ht="14.36309523792468" customHeight="1"/>
+    <row r="60" ht="14.36309523792468" customHeight="1"/>
+    <row r="61" ht="14.36309523792468" customHeight="1"/>
+    <row r="62" ht="14.36309523792468" customHeight="1"/>
+    <row r="63" ht="14.36309523792468" customHeight="1"/>
+    <row r="64" ht="14.36309523792468" customHeight="1"/>
+    <row r="65" ht="14.36309523792468" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>

</xml_diff>